<commit_message>
add preview of risk measures
</commit_message>
<xml_diff>
--- a/Inputs_data/NYCTRS_PlanInfo_AV2017.xlsx
+++ b/Inputs_data/NYCTRS_PlanInfo_AV2017.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\RSF_NYCTRS\Inputs_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0276A6B-4338-463A-A634-ADBF588A7746}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1769B71D-11AB-4979-A801-1B409B2397AE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="853" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="100">
   <si>
     <t>Notes</t>
   </si>
@@ -385,7 +385,7 @@
     <t>cp</t>
   </si>
   <si>
-    <t>K10</t>
+    <t>K11</t>
   </si>
 </sst>
 </file>
@@ -7643,7 +7643,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7766,7 +7766,7 @@
         <v>21</v>
       </c>
       <c r="H8" s="81">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="I8" s="59">
         <v>18</v>
@@ -7792,7 +7792,7 @@
         <v>14</v>
       </c>
       <c r="H9" s="81">
-        <v>0.125</v>
+        <v>0.1</v>
       </c>
       <c r="I9" s="59">
         <v>12</v>
@@ -7818,7 +7818,7 @@
         <v>14</v>
       </c>
       <c r="H10" s="81">
-        <v>0.125</v>
+        <v>0.1</v>
       </c>
       <c r="I10" s="59">
         <v>13</v>
@@ -7834,12 +7834,27 @@
       <c r="B11" s="52"/>
       <c r="C11" s="56"/>
       <c r="D11" s="57"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
+      <c r="E11" s="77">
+        <v>2015</v>
+      </c>
+      <c r="F11" s="81">
+        <v>0.125</v>
+      </c>
+      <c r="G11" s="59">
+        <v>14</v>
+      </c>
+      <c r="H11" s="81">
+        <v>0.1</v>
+      </c>
+      <c r="I11" s="59">
+        <v>14</v>
+      </c>
+      <c r="J11" s="80">
+        <v>0</v>
+      </c>
+      <c r="K11" s="60" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" s="52"/>

</xml_diff>

<commit_message>
add simple initial deferred returns
</commit_message>
<xml_diff>
--- a/Inputs_data/NYCTRS_PlanInfo_AV2017.xlsx
+++ b/Inputs_data/NYCTRS_PlanInfo_AV2017.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\RSF_NYCTRS\Inputs_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1769B71D-11AB-4979-A801-1B409B2397AE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B866F50-14C8-4D86-88DF-355AC6D47F05}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="853" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="853" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="44" r:id="rId1"/>
@@ -379,13 +379,13 @@
     <t>K8</t>
   </si>
   <si>
-    <t>D10</t>
-  </si>
-  <si>
     <t>cp</t>
   </si>
   <si>
     <t>K11</t>
+  </si>
+  <si>
+    <t>D11</t>
   </si>
 </sst>
 </file>
@@ -7642,8 +7642,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7680,7 +7680,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F3" s="30"/>
     </row>
@@ -7775,7 +7775,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="60" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -8156,8 +8156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8189,7 +8189,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
@@ -8221,7 +8221,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C7">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -8244,7 +8244,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C8">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -8267,7 +8267,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -8290,7 +8290,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C10">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -8308,6 +8308,12 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>2021</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
       <c r="I11" s="35"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add analysis of results
</commit_message>
<xml_diff>
--- a/Inputs_data/NYCTRS_PlanInfo_AV2017.xlsx
+++ b/Inputs_data/NYCTRS_PlanInfo_AV2017.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\RSF_NYCTRS\Inputs_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B866F50-14C8-4D86-88DF-355AC6D47F05}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40AF93A3-3346-4E9D-804D-9642B707D249}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="853" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" tabRatio="853" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="44" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="detective" sheetId="40" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="102">
   <si>
     <t>Notes</t>
   </si>
@@ -382,10 +383,16 @@
     <t>cp</t>
   </si>
   <si>
-    <t>K11</t>
-  </si>
-  <si>
     <t>D11</t>
+  </si>
+  <si>
+    <t>amort.type</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>L11</t>
   </si>
 </sst>
 </file>
@@ -4601,7 +4608,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>70</v>
       </c>
@@ -7642,8 +7649,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7658,6 +7665,7 @@
     <col min="8" max="8" width="32.28515625" style="33" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
     <col min="12" max="15" width="27.28515625" customWidth="1"/>
     <col min="16" max="19" width="14.5703125" customWidth="1"/>
   </cols>
@@ -7680,7 +7688,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F3" s="30"/>
     </row>
@@ -7750,6 +7758,9 @@
       <c r="K7" s="72" t="s">
         <v>48</v>
       </c>
+      <c r="L7" s="72" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C8" s="75" t="s">
@@ -7776,6 +7787,9 @@
       </c>
       <c r="K8" s="60" t="s">
         <v>97</v>
+      </c>
+      <c r="L8" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -7803,6 +7817,9 @@
       <c r="K9" s="60" t="s">
         <v>65</v>
       </c>
+      <c r="L9" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" s="52"/>
@@ -7829,6 +7846,9 @@
       <c r="K10" s="60" t="s">
         <v>65</v>
       </c>
+      <c r="L10" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" s="52"/>
@@ -7854,6 +7874,9 @@
       </c>
       <c r="K11" s="60" t="s">
         <v>65</v>
+      </c>
+      <c r="L11" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -8156,7 +8179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -8189,7 +8212,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>

</xml_diff>